<commit_message>
fixed MSTG version for link generation in checklists
</commit_message>
<xml_diff>
--- a/Checklists/Mobile_App_Security_Checklist-English_1.2.xlsx
+++ b/Checklists/Mobile_App_Security_Checklist-English_1.2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sven/PentestTools/OWASP/owasp-mstg/Checklists/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFFFC71E-9B03-054E-8685-8A50851AD211}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B97A55F9-A1B9-EB47-8051-CBEC824FD855}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" tabRatio="705" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="705" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1096" uniqueCount="400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1097" uniqueCount="401">
   <si>
     <r>
       <rPr>
@@ -1432,6 +1432,9 @@
     <t xml:space="preserve">The two rows above are used to construct the base for all hyperlinks in the Android and iOS checklists. 
 Adjust to your specific use case to update all hyperlinks to a specific version of the MSTG </t>
     <phoneticPr fontId="27"/>
+  </si>
+  <si>
+    <t>1.1.3-excel</t>
   </si>
 </sst>
 </file>
@@ -2357,35 +2360,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2409,42 +2413,13 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
   </cellStyles>
-  <dxfs count="14">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="10">
     <dxf>
       <fill>
         <patternFill>
@@ -3751,7 +3726,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:D50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
@@ -3766,46 +3741,46 @@
   <sheetData>
     <row r="1" spans="2:4" ht="8" customHeight="1"/>
     <row r="2" spans="2:4" ht="15.75" customHeight="1">
-      <c r="B2" s="126" t="s">
+      <c r="B2" s="120" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="126"/>
-      <c r="D2" s="126"/>
+      <c r="C2" s="120"/>
+      <c r="D2" s="120"/>
     </row>
     <row r="3" spans="2:4">
-      <c r="B3" s="126"/>
-      <c r="C3" s="126"/>
-      <c r="D3" s="126"/>
+      <c r="B3" s="120"/>
+      <c r="C3" s="120"/>
+      <c r="D3" s="120"/>
     </row>
     <row r="4" spans="2:4">
-      <c r="B4" s="126"/>
-      <c r="C4" s="126"/>
-      <c r="D4" s="126"/>
+      <c r="B4" s="120"/>
+      <c r="C4" s="120"/>
+      <c r="D4" s="120"/>
     </row>
     <row r="5" spans="2:4">
-      <c r="B5" s="126"/>
-      <c r="C5" s="126"/>
-      <c r="D5" s="126"/>
+      <c r="B5" s="120"/>
+      <c r="C5" s="120"/>
+      <c r="D5" s="120"/>
     </row>
     <row r="6" spans="2:4">
-      <c r="B6" s="126"/>
-      <c r="C6" s="126"/>
-      <c r="D6" s="126"/>
+      <c r="B6" s="120"/>
+      <c r="C6" s="120"/>
+      <c r="D6" s="120"/>
     </row>
     <row r="7" spans="2:4">
-      <c r="B7" s="126"/>
-      <c r="C7" s="126"/>
-      <c r="D7" s="126"/>
+      <c r="B7" s="120"/>
+      <c r="C7" s="120"/>
+      <c r="D7" s="120"/>
     </row>
     <row r="8" spans="2:4" hidden="1">
-      <c r="B8" s="126"/>
-      <c r="C8" s="126"/>
-      <c r="D8" s="126"/>
+      <c r="B8" s="120"/>
+      <c r="C8" s="120"/>
+      <c r="D8" s="120"/>
     </row>
     <row r="9" spans="2:4">
-      <c r="B9" s="123"/>
-      <c r="C9" s="123"/>
-      <c r="D9" s="123"/>
+      <c r="B9" s="121"/>
+      <c r="C9" s="121"/>
+      <c r="D9" s="121"/>
     </row>
     <row r="10" spans="2:4">
       <c r="B10" s="1" t="s">
@@ -3815,41 +3790,41 @@
       <c r="D10" s="3"/>
     </row>
     <row r="11" spans="2:4">
-      <c r="B11" s="127" t="s">
+      <c r="B11" s="122" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="127"/>
+      <c r="C11" s="122"/>
       <c r="D11" s="64">
         <v>1.2</v>
       </c>
     </row>
     <row r="12" spans="2:4">
-      <c r="B12" s="124" t="s">
+      <c r="B12" s="123" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="124"/>
+      <c r="C12" s="123"/>
       <c r="D12" s="4" t="str">
         <f>HYPERLINK(CONCATENATE( "https://github.com/OWASP/owasp-masvs/blob/", MASVS_VERSION, "/Document/"))</f>
         <v>https://github.com/OWASP/owasp-masvs/blob/1.2/Document/</v>
       </c>
     </row>
     <row r="13" spans="2:4">
-      <c r="B13" s="128" t="s">
+      <c r="B13" s="124" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="128"/>
-      <c r="D13" s="5">
-        <v>1.2</v>
+      <c r="C13" s="124"/>
+      <c r="D13" s="5" t="s">
+        <v>400</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="17">
-      <c r="B14" s="124" t="s">
+      <c r="B14" s="123" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="124"/>
+      <c r="C14" s="123"/>
       <c r="D14" s="6" t="str">
         <f>HYPERLINK(CONCATENATE( "https://github.com/OWASP/owasp-mstg/blob/", MSTG_VERSION, "/Document/"))</f>
-        <v>https://github.com/OWASP/owasp-mstg/blob/1.2/Document/</v>
+        <v>https://github.com/OWASP/owasp-mstg/blob/1.1.3-excel/Document/</v>
       </c>
     </row>
     <row r="15" spans="2:4" ht="32" customHeight="1">
@@ -3860,62 +3835,62 @@
       <c r="D15" s="125"/>
     </row>
     <row r="16" spans="2:4">
-      <c r="B16" s="121" t="s">
+      <c r="B16" s="126" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="121"/>
+      <c r="C16" s="126"/>
       <c r="D16" s="5"/>
     </row>
     <row r="17" spans="2:4">
-      <c r="B17" s="124" t="s">
+      <c r="B17" s="123" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="124"/>
+      <c r="C17" s="123"/>
       <c r="D17" s="5"/>
     </row>
     <row r="18" spans="2:4">
-      <c r="B18" s="121" t="s">
+      <c r="B18" s="126" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="121"/>
+      <c r="C18" s="126"/>
       <c r="D18" s="5"/>
     </row>
     <row r="19" spans="2:4">
-      <c r="B19" s="121" t="s">
+      <c r="B19" s="126" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="121"/>
+      <c r="C19" s="126"/>
       <c r="D19" s="5"/>
     </row>
     <row r="20" spans="2:4">
-      <c r="B20" s="121" t="s">
+      <c r="B20" s="126" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="121"/>
+      <c r="C20" s="126"/>
       <c r="D20" s="5"/>
     </row>
     <row r="21" spans="2:4">
-      <c r="B21" s="121" t="s">
+      <c r="B21" s="126" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="121"/>
+      <c r="C21" s="126"/>
       <c r="D21" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="70.5" customHeight="1">
-      <c r="B22" s="121" t="s">
+      <c r="B22" s="126" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="121"/>
+      <c r="C22" s="126"/>
       <c r="D22" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="23" spans="2:4">
-      <c r="B23" s="123"/>
-      <c r="C23" s="123"/>
-      <c r="D23" s="123"/>
+      <c r="B23" s="121"/>
+      <c r="C23" s="121"/>
+      <c r="D23" s="121"/>
     </row>
     <row r="24" spans="2:4">
       <c r="B24" s="7" t="s">
@@ -3932,37 +3907,37 @@
       <c r="D25" s="5"/>
     </row>
     <row r="26" spans="2:4">
-      <c r="B26" s="121" t="s">
+      <c r="B26" s="126" t="s">
         <v>18</v>
       </c>
-      <c r="C26" s="121"/>
+      <c r="C26" s="126"/>
       <c r="D26" s="5"/>
     </row>
     <row r="27" spans="2:4">
-      <c r="B27" s="121" t="s">
+      <c r="B27" s="126" t="s">
         <v>19</v>
       </c>
-      <c r="C27" s="121"/>
+      <c r="C27" s="126"/>
       <c r="D27" s="5"/>
     </row>
     <row r="28" spans="2:4">
-      <c r="B28" s="121" t="s">
+      <c r="B28" s="126" t="s">
         <v>20</v>
       </c>
-      <c r="C28" s="121"/>
+      <c r="C28" s="126"/>
       <c r="D28" s="5"/>
     </row>
     <row r="29" spans="2:4" ht="66" customHeight="1">
-      <c r="B29" s="122" t="s">
+      <c r="B29" s="127" t="s">
         <v>21</v>
       </c>
-      <c r="C29" s="122"/>
+      <c r="C29" s="127"/>
       <c r="D29" s="5"/>
     </row>
     <row r="30" spans="2:4">
-      <c r="B30" s="123"/>
-      <c r="C30" s="123"/>
-      <c r="D30" s="123"/>
+      <c r="B30" s="121"/>
+      <c r="C30" s="121"/>
+      <c r="D30" s="121"/>
     </row>
     <row r="31" spans="2:4">
       <c r="B31" s="7" t="s">
@@ -3979,37 +3954,37 @@
       <c r="D32" s="5"/>
     </row>
     <row r="33" spans="2:4">
-      <c r="B33" s="121" t="s">
+      <c r="B33" s="126" t="s">
         <v>23</v>
       </c>
-      <c r="C33" s="121"/>
+      <c r="C33" s="126"/>
       <c r="D33" s="5"/>
     </row>
     <row r="34" spans="2:4">
-      <c r="B34" s="121" t="s">
+      <c r="B34" s="126" t="s">
         <v>19</v>
       </c>
-      <c r="C34" s="121"/>
+      <c r="C34" s="126"/>
       <c r="D34" s="5"/>
     </row>
     <row r="35" spans="2:4">
-      <c r="B35" s="121" t="s">
+      <c r="B35" s="126" t="s">
         <v>20</v>
       </c>
-      <c r="C35" s="121"/>
+      <c r="C35" s="126"/>
       <c r="D35" s="5"/>
     </row>
     <row r="36" spans="2:4" ht="63" customHeight="1">
-      <c r="B36" s="122" t="s">
+      <c r="B36" s="127" t="s">
         <v>24</v>
       </c>
-      <c r="C36" s="122"/>
+      <c r="C36" s="127"/>
       <c r="D36" s="5"/>
     </row>
     <row r="37" spans="2:4">
-      <c r="B37" s="123"/>
-      <c r="C37" s="123"/>
-      <c r="D37" s="123"/>
+      <c r="B37" s="121"/>
+      <c r="C37" s="121"/>
+      <c r="D37" s="121"/>
     </row>
     <row r="38" spans="2:4">
       <c r="B38" s="7" t="s">
@@ -4019,117 +3994,87 @@
       <c r="D38" s="9"/>
     </row>
     <row r="39" spans="2:4">
-      <c r="B39" s="120"/>
-      <c r="C39" s="120"/>
-      <c r="D39" s="120"/>
+      <c r="B39" s="128"/>
+      <c r="C39" s="128"/>
+      <c r="D39" s="128"/>
     </row>
     <row r="40" spans="2:4">
-      <c r="B40" s="119" t="s">
+      <c r="B40" s="129" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="119"/>
+      <c r="C40" s="129"/>
       <c r="D40" s="12"/>
     </row>
     <row r="41" spans="2:4">
-      <c r="B41" s="119" t="s">
+      <c r="B41" s="129" t="s">
         <v>27</v>
       </c>
-      <c r="C41" s="119"/>
+      <c r="C41" s="129"/>
       <c r="D41" s="12"/>
     </row>
     <row r="42" spans="2:4">
-      <c r="B42" s="119" t="s">
+      <c r="B42" s="129" t="s">
         <v>28</v>
       </c>
-      <c r="C42" s="119"/>
+      <c r="C42" s="129"/>
       <c r="D42" s="12"/>
     </row>
     <row r="43" spans="2:4">
-      <c r="B43" s="119" t="s">
+      <c r="B43" s="129" t="s">
         <v>29</v>
       </c>
-      <c r="C43" s="119"/>
+      <c r="C43" s="129"/>
       <c r="D43" s="13"/>
     </row>
     <row r="44" spans="2:4">
-      <c r="B44" s="119" t="s">
+      <c r="B44" s="129" t="s">
         <v>30</v>
       </c>
-      <c r="C44" s="119"/>
+      <c r="C44" s="129"/>
       <c r="D44" s="12"/>
     </row>
     <row r="45" spans="2:4">
-      <c r="B45" s="120"/>
-      <c r="C45" s="120"/>
-      <c r="D45" s="120"/>
+      <c r="B45" s="128"/>
+      <c r="C45" s="128"/>
+      <c r="D45" s="128"/>
     </row>
     <row r="46" spans="2:4">
-      <c r="B46" s="119" t="s">
+      <c r="B46" s="129" t="s">
         <v>26</v>
       </c>
-      <c r="C46" s="119"/>
+      <c r="C46" s="129"/>
       <c r="D46" s="12"/>
     </row>
     <row r="47" spans="2:4">
-      <c r="B47" s="119" t="s">
+      <c r="B47" s="129" t="s">
         <v>27</v>
       </c>
-      <c r="C47" s="119"/>
+      <c r="C47" s="129"/>
       <c r="D47" s="12"/>
     </row>
     <row r="48" spans="2:4">
-      <c r="B48" s="119" t="s">
+      <c r="B48" s="129" t="s">
         <v>28</v>
       </c>
-      <c r="C48" s="119"/>
+      <c r="C48" s="129"/>
       <c r="D48" s="12"/>
     </row>
     <row r="49" spans="2:4">
-      <c r="B49" s="119" t="s">
+      <c r="B49" s="129" t="s">
         <v>29</v>
       </c>
-      <c r="C49" s="119"/>
+      <c r="C49" s="129"/>
       <c r="D49" s="13"/>
     </row>
     <row r="50" spans="2:4">
-      <c r="B50" s="119" t="s">
+      <c r="B50" s="129" t="s">
         <v>30</v>
       </c>
-      <c r="C50" s="119"/>
+      <c r="C50" s="129"/>
       <c r="D50" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="B2:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
     <mergeCell ref="B49:C49"/>
     <mergeCell ref="B50:C50"/>
     <mergeCell ref="B44:C44"/>
@@ -4137,6 +4082,36 @@
     <mergeCell ref="B46:C46"/>
     <mergeCell ref="B47:C47"/>
     <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B2:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
   </mergeCells>
   <phoneticPr fontId="27"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -4180,11 +4155,11 @@
       <c r="F3" s="17"/>
     </row>
     <row r="4" spans="2:24">
-      <c r="B4" s="130"/>
-      <c r="C4" s="130"/>
-      <c r="D4" s="130"/>
-      <c r="E4" s="130"/>
-      <c r="F4" s="130"/>
+      <c r="B4" s="131"/>
+      <c r="C4" s="131"/>
+      <c r="D4" s="131"/>
+      <c r="E4" s="131"/>
+      <c r="F4" s="131"/>
     </row>
     <row r="5" spans="2:24" ht="16" customHeight="1">
       <c r="B5" s="18"/>
@@ -4199,16 +4174,16 @@
       <c r="D6" s="19"/>
       <c r="E6" s="19"/>
       <c r="F6" s="19"/>
-      <c r="G6" s="131" t="s">
+      <c r="G6" s="132" t="s">
         <v>32</v>
       </c>
-      <c r="H6" s="131"/>
-      <c r="I6" s="131"/>
-      <c r="V6" s="131" t="s">
+      <c r="H6" s="132"/>
+      <c r="I6" s="132"/>
+      <c r="V6" s="132" t="s">
         <v>32</v>
       </c>
-      <c r="W6" s="131"/>
-      <c r="X6" s="131"/>
+      <c r="W6" s="132"/>
+      <c r="X6" s="132"/>
     </row>
     <row r="7" spans="2:24">
       <c r="B7" s="20"/>
@@ -4223,18 +4198,18 @@
       <c r="D8" s="18"/>
       <c r="E8" s="18"/>
       <c r="F8" s="18"/>
-      <c r="G8" s="132">
+      <c r="G8" s="133">
         <f>AVERAGE(G43:G50)*5</f>
         <v>0</v>
       </c>
-      <c r="H8" s="132"/>
-      <c r="I8" s="132"/>
-      <c r="V8" s="132">
+      <c r="H8" s="133"/>
+      <c r="I8" s="133"/>
+      <c r="V8" s="133">
         <f>AVERAGE(K43:K50)*5</f>
         <v>0</v>
       </c>
-      <c r="W8" s="132"/>
-      <c r="X8" s="132"/>
+      <c r="W8" s="133"/>
+      <c r="X8" s="133"/>
     </row>
     <row r="9" spans="2:24" ht="91" customHeight="1">
       <c r="B9" s="19"/>
@@ -4242,12 +4217,12 @@
       <c r="D9" s="19"/>
       <c r="E9" s="19"/>
       <c r="F9" s="19"/>
-      <c r="G9" s="132"/>
-      <c r="H9" s="132"/>
-      <c r="I9" s="132"/>
-      <c r="V9" s="132"/>
-      <c r="W9" s="132"/>
-      <c r="X9" s="132"/>
+      <c r="G9" s="133"/>
+      <c r="H9" s="133"/>
+      <c r="I9" s="133"/>
+      <c r="V9" s="133"/>
+      <c r="W9" s="133"/>
+      <c r="X9" s="133"/>
     </row>
     <row r="10" spans="2:24" ht="16.5" customHeight="1">
       <c r="B10" s="20"/>
@@ -4255,12 +4230,12 @@
       <c r="D10" s="20"/>
       <c r="E10" s="20"/>
       <c r="F10" s="20"/>
-      <c r="G10" s="132"/>
-      <c r="H10" s="132"/>
-      <c r="I10" s="132"/>
-      <c r="V10" s="132"/>
-      <c r="W10" s="132"/>
-      <c r="X10" s="132"/>
+      <c r="G10" s="133"/>
+      <c r="H10" s="133"/>
+      <c r="I10" s="133"/>
+      <c r="V10" s="133"/>
+      <c r="W10" s="133"/>
+      <c r="X10" s="133"/>
     </row>
     <row r="11" spans="2:24" ht="17.25" customHeight="1">
       <c r="B11" s="20"/>
@@ -4268,19 +4243,19 @@
       <c r="D11" s="20"/>
       <c r="E11" s="20"/>
       <c r="F11" s="20"/>
-      <c r="G11" s="132"/>
-      <c r="H11" s="132"/>
-      <c r="I11" s="132"/>
-      <c r="V11" s="132"/>
-      <c r="W11" s="132"/>
-      <c r="X11" s="132"/>
+      <c r="G11" s="133"/>
+      <c r="H11" s="133"/>
+      <c r="I11" s="133"/>
+      <c r="V11" s="133"/>
+      <c r="W11" s="133"/>
+      <c r="X11" s="133"/>
     </row>
     <row r="12" spans="2:24" ht="16" customHeight="1">
-      <c r="B12" s="133"/>
-      <c r="C12" s="133"/>
-      <c r="D12" s="133"/>
-      <c r="E12" s="133"/>
-      <c r="F12" s="133"/>
+      <c r="B12" s="134"/>
+      <c r="C12" s="134"/>
+      <c r="D12" s="134"/>
+      <c r="E12" s="134"/>
+      <c r="F12" s="134"/>
     </row>
     <row r="13" spans="2:24">
       <c r="B13" s="21"/>
@@ -4304,11 +4279,11 @@
       <c r="F15" s="20"/>
     </row>
     <row r="16" spans="2:24" ht="16" customHeight="1">
-      <c r="B16" s="133"/>
-      <c r="C16" s="133"/>
-      <c r="D16" s="133"/>
-      <c r="E16" s="133"/>
-      <c r="F16" s="133"/>
+      <c r="B16" s="134"/>
+      <c r="C16" s="134"/>
+      <c r="D16" s="134"/>
+      <c r="E16" s="134"/>
+      <c r="F16" s="134"/>
     </row>
     <row r="17" spans="2:6">
       <c r="B17" s="21"/>
@@ -4361,18 +4336,18 @@
     </row>
     <row r="35" spans="3:11" ht="15.75" customHeight="1"/>
     <row r="41" spans="3:11">
-      <c r="D41" s="129" t="s">
+      <c r="D41" s="130" t="s">
         <v>34</v>
       </c>
-      <c r="E41" s="129"/>
-      <c r="F41" s="129"/>
-      <c r="G41" s="129"/>
-      <c r="H41" s="129" t="s">
+      <c r="E41" s="130"/>
+      <c r="F41" s="130"/>
+      <c r="G41" s="130"/>
+      <c r="H41" s="130" t="s">
         <v>35</v>
       </c>
-      <c r="I41" s="129"/>
-      <c r="J41" s="129"/>
-      <c r="K41" s="129"/>
+      <c r="I41" s="130"/>
+      <c r="J41" s="130"/>
+      <c r="K41" s="130"/>
     </row>
     <row r="42" spans="3:11">
       <c r="D42" s="25" t="s">
@@ -4719,7 +4694,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F14">
-    <cfRule type="expression" dxfId="13" priority="3">
+    <cfRule type="expression" dxfId="9" priority="3">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4733,7 +4708,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F18">
-    <cfRule type="expression" dxfId="12" priority="5">
+    <cfRule type="expression" dxfId="8" priority="5">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4747,7 +4722,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AMK94"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="16"/>
   <cols>
@@ -4768,18 +4745,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="19">
-      <c r="B1" s="134" t="s">
+      <c r="B1" s="135" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="134"/>
-      <c r="D1" s="134"/>
-      <c r="E1" s="134"/>
-      <c r="F1" s="134"/>
-      <c r="G1" s="134"/>
-      <c r="H1" s="134"/>
-      <c r="I1" s="134"/>
-      <c r="J1" s="134"/>
-      <c r="K1" s="134"/>
+      <c r="C1" s="135"/>
+      <c r="D1" s="135"/>
+      <c r="E1" s="135"/>
+      <c r="F1" s="135"/>
+      <c r="G1" s="135"/>
+      <c r="H1" s="135"/>
+      <c r="I1" s="135"/>
+      <c r="J1" s="135"/>
+      <c r="K1" s="135"/>
     </row>
     <row r="2" spans="2:11">
       <c r="B2" s="67"/>
@@ -4812,10 +4789,10 @@
       <c r="G3" s="63" t="s">
         <v>54</v>
       </c>
-      <c r="H3" s="135" t="s">
+      <c r="H3" s="136" t="s">
         <v>55</v>
       </c>
-      <c r="I3" s="135"/>
+      <c r="I3" s="136"/>
       <c r="J3" s="34"/>
       <c r="K3" s="35" t="s">
         <v>56</v>
@@ -7506,11 +7483,11 @@
       <c r="G3" s="63" t="s">
         <v>54</v>
       </c>
-      <c r="H3" s="135" t="s">
+      <c r="H3" s="136" t="s">
         <v>55</v>
       </c>
-      <c r="I3" s="135"/>
-      <c r="J3" s="135"/>
+      <c r="I3" s="136"/>
+      <c r="J3" s="136"/>
       <c r="K3" s="35" t="s">
         <v>56</v>
       </c>
@@ -9572,22 +9549,22 @@
   </mergeCells>
   <phoneticPr fontId="27"/>
   <conditionalFormatting sqref="M1:M1048576">
-    <cfRule type="containsText" dxfId="11" priority="2" operator="containsText" text="0x05">
+    <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="0x05">
       <formula>NOT(ISERROR(SEARCH("0x05",M1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H28 H33:H1048576">
-    <cfRule type="containsText" dxfId="10" priority="3" operator="containsText" text="0x05">
+    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="0x05">
       <formula>NOT(ISERROR(SEARCH("0x05",H1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J6">
-    <cfRule type="containsText" dxfId="9" priority="4" operator="containsText" text="0x05">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="0x05">
       <formula>NOT(ISERROR(SEARCH("0x05",J6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6">
-    <cfRule type="containsText" dxfId="8" priority="5" operator="containsText" text="0x05">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="0x05">
       <formula>NOT(ISERROR(SEARCH("0x05",I6)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9756,7 +9733,7 @@
       <c r="F8" s="111" t="s">
         <v>75</v>
       </c>
-      <c r="G8" s="137" t="str">
+      <c r="G8" s="119" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06j-Testing-Resiliency-Against-Reverse-Engineering.md#testing-reverse-engineering-tools-detection-mstg-resilience-4"),"Testing Reverse Engineering Tools Detection (MSTG-RESILIENCE-4)")</f>
         <v>Testing Reverse Engineering Tools Detection (MSTG-RESILIENCE-4)</v>
       </c>
@@ -9778,7 +9755,7 @@
       <c r="F9" s="111" t="s">
         <v>75</v>
       </c>
-      <c r="G9" s="137" t="str">
+      <c r="G9" s="119" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06j-Testing-Resiliency-Against-Reverse-Engineering.md#testing-emulator-detection-mstg-resilience-5"),"Testing Emulator Detection (MSTG-RESILIENCE-5)")</f>
         <v>Testing Emulator Detection (MSTG-RESILIENCE-5)</v>
       </c>
@@ -9800,7 +9777,7 @@
       <c r="F10" s="111" t="s">
         <v>75</v>
       </c>
-      <c r="G10" s="137"/>
+      <c r="G10" s="119"/>
       <c r="H10" s="112"/>
     </row>
     <row r="11" spans="2:8" ht="32">
@@ -9861,7 +9838,7 @@
       <c r="F13" s="111" t="s">
         <v>75</v>
       </c>
-      <c r="G13" s="137" t="str">
+      <c r="G13" s="119" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06j-Testing-Resiliency-Against-Reverse-Engineering.md#testing-obfuscation-mstg-resilience-9"),"Testing Obfuscation (MSTG-RESILIENCE-9)")</f>
         <v>Testing Obfuscation (MSTG-RESILIENCE-9)</v>
       </c>
@@ -10127,12 +10104,12 @@
   </sheetData>
   <phoneticPr fontId="27"/>
   <conditionalFormatting sqref="G11">
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="0x05">
+    <cfRule type="containsText" dxfId="3" priority="5" operator="containsText" text="0x05">
       <formula>NOT(ISERROR(SEARCH("0x05",G11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G12">
-    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="0x05">
+    <cfRule type="containsText" dxfId="2" priority="6" operator="containsText" text="0x05">
       <formula>NOT(ISERROR(SEARCH("0x05",G12)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10176,10 +10153,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="136" t="s">
+      <c r="A1" s="137" t="s">
         <v>309</v>
       </c>
-      <c r="B1" s="136"/>
+      <c r="B1" s="137"/>
       <c r="C1" s="50"/>
       <c r="D1" s="32"/>
       <c r="E1" s="32"/>

</xml_diff>